<commit_message>
formatting boxplots for Results outline
</commit_message>
<xml_diff>
--- a/species2.xlsx
+++ b/species2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slane84\OneDrive - The University Of British Columbia\Documents\Dissertation\HabitatRecovery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39A8934-3D91-4EC2-A090-5BA4CB8D61A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{E39A8934-3D91-4EC2-A090-5BA4CB8D61A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{FFD49679-91E0-42B5-BDA8-D50B36926BC2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{BBB8E670-FD30-408F-B694-695B488B79B0}"/>
   </bookViews>
@@ -183,12 +183,6 @@
     <t>Juncus balticus</t>
   </si>
   <si>
-    <t>Cirsium sp</t>
-  </si>
-  <si>
-    <t>cirsp</t>
-  </si>
-  <si>
     <t>jubu</t>
   </si>
   <si>
@@ -262,6 +256,12 @@
   </si>
   <si>
     <t>sama</t>
+  </si>
+  <si>
+    <t>Sonchus asper</t>
+  </si>
+  <si>
+    <t>soas</t>
   </si>
 </sst>
 </file>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BD2547-4DF3-41B2-AFC9-3253A2A5901E}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -661,7 +661,7 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
@@ -684,7 +684,7 @@
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
@@ -707,7 +707,7 @@
         <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
         <v>29</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -730,7 +730,7 @@
         <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
@@ -753,7 +753,7 @@
         <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
@@ -767,19 +767,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
         <v>27</v>
@@ -799,7 +799,7 @@
         <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -822,7 +822,7 @@
         <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -845,7 +845,7 @@
         <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -868,7 +868,7 @@
         <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
@@ -891,7 +891,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
@@ -905,16 +905,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
         <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -937,7 +937,7 @@
         <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
@@ -960,7 +960,7 @@
         <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
         <v>26</v>
@@ -983,7 +983,7 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
@@ -1006,7 +1006,7 @@
         <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -1020,16 +1020,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
         <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -1043,16 +1043,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
         <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
@@ -1075,7 +1075,7 @@
         <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
         <v>26</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
         <v>16</v>
@@ -1098,7 +1098,7 @@
         <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
@@ -1121,7 +1121,7 @@
         <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
         <v>26</v>
@@ -1144,7 +1144,7 @@
         <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
         <v>26</v>
@@ -1167,7 +1167,7 @@
         <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
         <v>29</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
@@ -1190,7 +1190,7 @@
         <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E25" t="s">
         <v>29</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
@@ -1213,7 +1213,7 @@
         <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E26" t="s">
         <v>29</v>
@@ -1227,22 +1227,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
         <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G27" t="s">
         <v>37</v>
@@ -1250,16 +1250,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
         <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
         <v>29</v>
@@ -1273,16 +1273,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29" t="s">
         <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
         <v>29</v>
@@ -1296,16 +1296,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
         <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
         <v>29</v>
@@ -1327,6 +1327,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100483727557648AA40B029C215891F95C5" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d36f379eec1cf084072dcf956aecbcf8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8c008993-a31f-4b40-b1f3-88dd9c6e1924" xmlns:ns4="360018dd-41eb-4458-b1d4-4b46a95a2b02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd1f472f1ef3281fe4dbeb8213942d38" ns3:_="" ns4:_="">
     <xsd:import namespace="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
@@ -1555,22 +1570,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C816B061-1CDD-439F-8C9F-29C9EF4FB231}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
+    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CBD582-CD76-4265-9BA2-35ECC89DA4D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34E72DEF-7AF1-4F07-B46B-983AB5556665}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1587,29 +1612,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CBD582-CD76-4265-9BA2-35ECC89DA4D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C816B061-1CDD-439F-8C9F-29C9EF4FB231}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>